<commit_message>
Fix Epa compare report
</commit_message>
<xml_diff>
--- a/report_template/epa_compare.xlsx
+++ b/report_template/epa_compare.xlsx
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>FPG</t>
-  </si>
-  <si>
-    <t>二氧化硫</t>
   </si>
   <si>
     <t>EPA</t>
@@ -113,6 +110,10 @@
   </si>
   <si>
     <t>人工註記</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>風速</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -295,36 +296,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -333,6 +304,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,11 +463,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="437436288"/>
-        <c:axId val="437436680"/>
+        <c:axId val="444020272"/>
+        <c:axId val="444020664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="437436288"/>
+        <c:axId val="444020272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="437436680"/>
+        <c:crossAx val="444020664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -502,7 +503,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="437436680"/>
+        <c:axId val="444020664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -534,7 +535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="437436288"/>
+        <c:crossAx val="444020272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="90"/>
@@ -671,11 +672,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="431889720"/>
-        <c:axId val="574999120"/>
+        <c:axId val="444021840"/>
+        <c:axId val="444022624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="431889720"/>
+        <c:axId val="444021840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -703,7 +704,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574999120"/>
+        <c:crossAx val="444022624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -711,7 +712,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574999120"/>
+        <c:axId val="444022624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,7 +742,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431889720"/>
+        <c:crossAx val="444021840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -873,11 +874,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="574996768"/>
-        <c:axId val="574997160"/>
+        <c:axId val="444024192"/>
+        <c:axId val="444026544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="574996768"/>
+        <c:axId val="444024192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,7 +906,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574997160"/>
+        <c:crossAx val="444026544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -913,7 +914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574997160"/>
+        <c:axId val="444026544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,7 +944,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574996768"/>
+        <c:crossAx val="444024192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1075,11 +1076,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="574998728"/>
-        <c:axId val="574999512"/>
+        <c:axId val="445684256"/>
+        <c:axId val="445693664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="574998728"/>
+        <c:axId val="445684256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,7 +1108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574999512"/>
+        <c:crossAx val="445693664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1115,7 +1116,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574999512"/>
+        <c:axId val="445693664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,7 +1146,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574998728"/>
+        <c:crossAx val="445684256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1277,11 +1278,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="437439816"/>
-        <c:axId val="431890896"/>
+        <c:axId val="445683864"/>
+        <c:axId val="445691312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="437439816"/>
+        <c:axId val="445683864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,7 +1310,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431890896"/>
+        <c:crossAx val="445691312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1317,7 +1318,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="431890896"/>
+        <c:axId val="445691312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,7 +1348,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="437439816"/>
+        <c:crossAx val="445683864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1483,11 +1484,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="574979120"/>
-        <c:axId val="574982648"/>
+        <c:axId val="445692096"/>
+        <c:axId val="445692488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="574979120"/>
+        <c:axId val="445692096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1515,7 +1516,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574982648"/>
+        <c:crossAx val="445692488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1523,7 +1524,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574982648"/>
+        <c:axId val="445692488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1553,7 +1554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574979120"/>
+        <c:crossAx val="445692096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1697,11 +1698,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="574981472"/>
-        <c:axId val="574980296"/>
+        <c:axId val="445687784"/>
+        <c:axId val="445689744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="574981472"/>
+        <c:axId val="445687784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1729,7 +1730,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574980296"/>
+        <c:crossAx val="445689744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1737,7 +1738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574980296"/>
+        <c:axId val="445689744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1767,7 +1768,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574981472"/>
+        <c:crossAx val="445687784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1874,11 +1875,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="574980688"/>
-        <c:axId val="574979512"/>
+        <c:axId val="445688568"/>
+        <c:axId val="445693272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="574980688"/>
+        <c:axId val="445688568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1906,7 +1907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574979512"/>
+        <c:crossAx val="445693272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1914,7 +1915,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574979512"/>
+        <c:axId val="445693272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1944,7 +1945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574980688"/>
+        <c:crossAx val="445688568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2051,11 +2052,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="574982256"/>
-        <c:axId val="574997944"/>
+        <c:axId val="445686216"/>
+        <c:axId val="445688960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="574982256"/>
+        <c:axId val="445686216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2084,7 +2085,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574997944"/>
+        <c:crossAx val="445688960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2092,7 +2093,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574997944"/>
+        <c:axId val="445688960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2122,7 +2123,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="574982256"/>
+        <c:crossAx val="445686216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2708,7 +2709,7 @@
   <dimension ref="A1:AC137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2718,200 +2719,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
     </row>
     <row r="2" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
     </row>
     <row r="3" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="L3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+    </row>
+    <row r="4" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21">
+        <v>0</v>
+      </c>
+      <c r="D4" s="21">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21">
+        <v>2</v>
+      </c>
+      <c r="F4" s="21">
+        <v>3</v>
+      </c>
+      <c r="G4" s="21">
+        <v>4</v>
+      </c>
+      <c r="H4" s="21">
+        <v>5</v>
+      </c>
+      <c r="I4" s="21">
+        <v>6</v>
+      </c>
+      <c r="J4" s="21">
+        <v>7</v>
+      </c>
+      <c r="K4" s="21">
+        <v>8</v>
+      </c>
+      <c r="L4" s="21">
+        <v>9</v>
+      </c>
+      <c r="M4" s="21">
+        <v>10</v>
+      </c>
+      <c r="N4" s="21">
+        <v>11</v>
+      </c>
+      <c r="O4" s="21">
+        <v>12</v>
+      </c>
+      <c r="P4" s="21">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="21">
+        <v>14</v>
+      </c>
+      <c r="R4" s="21">
+        <v>15</v>
+      </c>
+      <c r="S4" s="21">
+        <v>16</v>
+      </c>
+      <c r="T4" s="21">
+        <v>17</v>
+      </c>
+      <c r="U4" s="21">
+        <v>18</v>
+      </c>
+      <c r="V4" s="21">
+        <v>19</v>
+      </c>
+      <c r="W4" s="21">
+        <v>20</v>
+      </c>
+      <c r="X4" s="21">
+        <v>21</v>
+      </c>
+      <c r="Y4" s="21">
         <v>22</v>
       </c>
-      <c r="M3" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-    </row>
-    <row r="4" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13">
-        <v>0</v>
-      </c>
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13">
-        <v>2</v>
-      </c>
-      <c r="F4" s="13">
-        <v>3</v>
-      </c>
-      <c r="G4" s="13">
-        <v>4</v>
-      </c>
-      <c r="H4" s="13">
-        <v>5</v>
-      </c>
-      <c r="I4" s="13">
-        <v>6</v>
-      </c>
-      <c r="J4" s="13">
-        <v>7</v>
-      </c>
-      <c r="K4" s="13">
-        <v>8</v>
-      </c>
-      <c r="L4" s="13">
-        <v>9</v>
-      </c>
-      <c r="M4" s="13">
-        <v>10</v>
-      </c>
-      <c r="N4" s="13">
-        <v>11</v>
-      </c>
-      <c r="O4" s="13">
-        <v>12</v>
-      </c>
-      <c r="P4" s="13">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="13">
-        <v>14</v>
-      </c>
-      <c r="R4" s="13">
-        <v>15</v>
-      </c>
-      <c r="S4" s="13">
-        <v>16</v>
-      </c>
-      <c r="T4" s="13">
-        <v>17</v>
-      </c>
-      <c r="U4" s="13">
-        <v>18</v>
-      </c>
-      <c r="V4" s="13">
-        <v>19</v>
-      </c>
-      <c r="W4" s="13">
-        <v>20</v>
-      </c>
-      <c r="X4" s="13">
-        <v>21</v>
-      </c>
-      <c r="Y4" s="13">
-        <v>22</v>
-      </c>
-      <c r="Z4" s="13">
+      <c r="Z4" s="21">
         <v>23</v>
       </c>
-      <c r="AA4" s="18" t="s">
+      <c r="AA4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AB4" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC4" s="13" t="s">
+      <c r="AC4" s="21" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2922,33 +2923,33 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="13"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="21"/>
     </row>
     <row r="6" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
@@ -2988,7 +2989,7 @@
     <row r="7" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -3020,7 +3021,7 @@
     </row>
     <row r="8" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -3056,7 +3057,7 @@
     <row r="9" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3088,7 +3089,7 @@
     </row>
     <row r="10" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -3124,7 +3125,7 @@
     <row r="11" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -3156,7 +3157,7 @@
     </row>
     <row r="12" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
@@ -3192,7 +3193,7 @@
     <row r="13" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3224,7 +3225,7 @@
     </row>
     <row r="14" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>9</v>
@@ -3260,7 +3261,7 @@
     <row r="15" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3292,7 +3293,7 @@
     </row>
     <row r="16" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
@@ -3328,7 +3329,7 @@
     <row r="17" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -3360,7 +3361,7 @@
     </row>
     <row r="18" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
@@ -3396,7 +3397,7 @@
     <row r="19" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3428,7 +3429,7 @@
     </row>
     <row r="20" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>9</v>
@@ -3464,7 +3465,7 @@
     <row r="21" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -3495,254 +3496,254 @@
       <c r="AC21" s="5"/>
     </row>
     <row r="22" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
-      <c r="AA22" s="15"/>
-      <c r="AB22" s="15"/>
-      <c r="AC22" s="15"/>
+      <c r="A22" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="20"/>
+      <c r="AA22" s="20"/>
+      <c r="AB22" s="20"/>
+      <c r="AC22" s="20"/>
     </row>
     <row r="23" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
-      <c r="AA23" s="15"/>
-      <c r="AB23" s="15"/>
-      <c r="AC23" s="15"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="20"/>
+      <c r="AA23" s="20"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="20"/>
     </row>
     <row r="24" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="15"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="15"/>
-      <c r="Z24" s="15"/>
-      <c r="AA24" s="15"/>
-      <c r="AB24" s="15"/>
-      <c r="AC24" s="15"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="20"/>
+      <c r="AA24" s="20"/>
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="20"/>
     </row>
     <row r="25" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
-      <c r="U25" s="15"/>
-      <c r="V25" s="15"/>
-      <c r="W25" s="15"/>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="15"/>
-      <c r="Z25" s="15"/>
-      <c r="AA25" s="15"/>
-      <c r="AB25" s="15"/>
-      <c r="AC25" s="15"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="20"/>
+      <c r="U25" s="20"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="20"/>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="20"/>
+      <c r="Z25" s="20"/>
+      <c r="AA25" s="20"/>
+      <c r="AB25" s="20"/>
+      <c r="AC25" s="20"/>
     </row>
     <row r="26" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
-      <c r="V26" s="14"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="14"/>
-      <c r="Y26" s="14"/>
-      <c r="Z26" s="14"/>
-      <c r="AA26" s="14"/>
-      <c r="AB26" s="14"/>
-      <c r="AC26" s="14"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="19"/>
+      <c r="Y26" s="19"/>
+      <c r="Z26" s="19"/>
+      <c r="AA26" s="19"/>
+      <c r="AB26" s="19"/>
+      <c r="AC26" s="19"/>
     </row>
     <row r="27" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="14"/>
-      <c r="AB27" s="14"/>
-      <c r="AC27" s="14"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="19"/>
+      <c r="AC27" s="19"/>
     </row>
     <row r="28" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-      <c r="V28" s="14"/>
-      <c r="W28" s="14"/>
-      <c r="X28" s="14"/>
-      <c r="Y28" s="14"/>
-      <c r="Z28" s="14"/>
-      <c r="AA28" s="14"/>
-      <c r="AB28" s="14"/>
-      <c r="AC28" s="14"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="19"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="19"/>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="19"/>
+      <c r="AC28" s="19"/>
     </row>
     <row r="29" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="14"/>
-      <c r="V29" s="14"/>
-      <c r="W29" s="14"/>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="14"/>
-      <c r="Z29" s="14"/>
-      <c r="AA29" s="14"/>
-      <c r="AB29" s="14"/>
-      <c r="AC29" s="14"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="19"/>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="19"/>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
@@ -6777,6 +6778,45 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="A1:AC1"/>
+    <mergeCell ref="A2:X2"/>
+    <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="Y3:AC3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="B22:AC29"/>
+    <mergeCell ref="A41:X41"/>
+    <mergeCell ref="Y41:AC41"/>
+    <mergeCell ref="AC4:AC5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="X4:X5"/>
+    <mergeCell ref="Y4:Y5"/>
+    <mergeCell ref="Z4:Z5"/>
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="AA4:AA5"/>
     <mergeCell ref="AB4:AB5"/>
     <mergeCell ref="A136:K136"/>
@@ -6793,45 +6833,6 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A29"/>
-    <mergeCell ref="B22:AC29"/>
-    <mergeCell ref="A41:X41"/>
-    <mergeCell ref="Y41:AC41"/>
-    <mergeCell ref="AC4:AC5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="V4:V5"/>
-    <mergeCell ref="W4:W5"/>
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="Y4:Y5"/>
-    <mergeCell ref="Z4:Z5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A1:AC1"/>
-    <mergeCell ref="A2:X2"/>
-    <mergeCell ref="Y2:AC2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="Y3:AC3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>